<commit_message>
se implementa scripts de HU crediágil en consulta de saldos por producto
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/saldosporproducto/saldos_por_producto.xlsx
+++ b/SVP/src/test/resources/datadriven/saldosporproducto/saldos_por_producto.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Todo1\Automatizacion\svp-rediseno-personas-web-tests-bdd-screenplay\SVP\src\test\resources\datadriven\saldosporproducto\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -20,7 +15,7 @@
     <sheet name="Crediagil" sheetId="8" r:id="rId6"/>
     <sheet name="Listas" sheetId="2" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +33,7 @@
     <author>Usuario</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +86,7 @@
     <author>Usuario</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +139,7 @@
     <author>Usuario</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +191,7 @@
     <author>Usuario</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -210,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -224,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -248,7 +243,7 @@
     <author>Usuario</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -262,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -276,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +295,7 @@
     <author>Usuario</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -314,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -328,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -347,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="79">
   <si>
     <t>Orientacion</t>
   </si>
@@ -409,9 +404,6 @@
     <t>7</t>
   </si>
   <si>
-    <t>OSVPPRU10</t>
-  </si>
-  <si>
     <t>854124014</t>
   </si>
   <si>
@@ -478,9 +470,6 @@
     <t>Inversión virtual visible y fondo de invercion oculto</t>
   </si>
   <si>
-    <t xml:space="preserve">Crediagil ocultas </t>
-  </si>
-  <si>
     <t>Sin cuentas</t>
   </si>
   <si>
@@ -575,6 +564,21 @@
   </si>
   <si>
     <t>0935000000538, 0935000000832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chipote95 </t>
+  </si>
+  <si>
+    <t>406-762740-18</t>
+  </si>
+  <si>
+    <t>OSVPPRU30</t>
+  </si>
+  <si>
+    <t>406-757950-06,406-757950-24,406-757950-25,406-157950-05</t>
+  </si>
+  <si>
+    <t>29281026324,10001263181</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1046,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1056,7 +1060,7 @@
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1105,25 +1109,25 @@
         <v>2</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="P1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="20" customFormat="1" ht="120">
@@ -1138,7 +1142,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="21"/>
       <c r="G2" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H2" s="23">
         <v>1234</v>
@@ -1148,23 +1152,23 @@
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M2" s="15">
         <v>29281023956</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O2" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P2" s="9"/>
       <c r="Q2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1179,7 +1183,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1189,17 +1193,17 @@
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1214,7 +1218,7 @@
       <c r="E4" s="9"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1229,10 +1233,10 @@
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1265,7 +1269,7 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
@@ -1307,25 +1311,25 @@
         <v>2</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="P1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1340,7 +1344,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1350,7 +1354,7 @@
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="3"/>
@@ -1358,7 +1362,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1373,7 +1377,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1388,10 +1392,10 @@
       <c r="N3" s="3"/>
       <c r="O3" s="4"/>
       <c r="P3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1406,7 +1410,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1417,14 +1421,14 @@
       <c r="J4" s="7"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1457,7 +1461,7 @@
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
@@ -1497,25 +1501,25 @@
         <v>2</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="P1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1530,7 +1534,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
       <c r="G2" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -1541,14 +1545,14 @@
       <c r="J2" s="4"/>
       <c r="K2" s="3"/>
       <c r="L2" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="4"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1563,7 +1567,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1578,10 +1582,10 @@
       <c r="N3" s="3"/>
       <c r="O3" s="4"/>
       <c r="P3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1596,7 +1600,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1606,7 +1610,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1614,7 +1618,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1643,7 +1647,7 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1684,25 +1688,25 @@
         <v>2</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="P1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1731,7 +1735,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1745,10 +1749,10 @@
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
       <c r="F3" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1763,10 +1767,10 @@
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
       <c r="P3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1781,7 +1785,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="12"/>
       <c r="G4" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H4" s="11">
         <v>1234</v>
@@ -1791,7 +1795,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1799,7 +1803,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1828,11 +1832,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
@@ -1876,25 +1880,25 @@
         <v>2</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="P1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1923,7 +1927,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1938,7 +1942,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -1953,10 +1957,10 @@
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
       <c r="P3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1984,10 +1988,10 @@
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -2015,10 +2019,10 @@
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2033,7 +2037,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="12"/>
       <c r="G6" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H6" s="11">
         <v>1234</v>
@@ -2046,12 +2050,12 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="165">
@@ -2065,10 +2069,10 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H7" s="19">
         <v>1234</v>
@@ -2078,21 +2082,21 @@
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>62</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="16">
         <v>12700025033</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2107,7 +2111,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="12"/>
       <c r="G8" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H8" s="11">
         <v>1234</v>
@@ -2117,7 +2121,7 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -2125,7 +2129,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2155,17 +2159,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="63.7109375" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.85546875" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -2202,25 +2207,25 @@
         <v>2</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="P1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -2234,10 +2239,10 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="H2" s="11">
         <v>1234</v>
@@ -2246,16 +2251,18 @@
         <v>1234</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="K2" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2263,16 +2270,14 @@
         <v>13</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="8" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="H3" s="11">
         <v>1234</v>
@@ -2280,67 +2285,26 @@
       <c r="I3" s="11">
         <v>1234</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>43</v>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="M3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="11">
-        <v>1234</v>
-      </c>
-      <c r="I4" s="11">
-        <v>1234</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="13"/>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="N8" s="14"/>
+      <c r="A4" s="13"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="N7" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2353,7 +2317,7 @@
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B4</xm:sqref>
+          <xm:sqref>B2:B3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2367,7 +2331,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
se ajustan scripts de saldos por producto y se implementan mapeos solicitados por banco
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/saldosporproducto/saldos_por_producto.xlsx
+++ b/SVP/src/test/resources/datadriven/saldosporproducto/saldos_por_producto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="3" r:id="rId1"/>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="87">
   <si>
     <t>Orientacion</t>
   </si>
@@ -579,6 +579,30 @@
   </si>
   <si>
     <t>29281026324,10001263181</t>
+  </si>
+  <si>
+    <t>TARJETAS</t>
+  </si>
+  <si>
+    <t>CUENTAS</t>
+  </si>
+  <si>
+    <t>CREDITOS</t>
+  </si>
+  <si>
+    <t>productos</t>
+  </si>
+  <si>
+    <t>INVERSIONES</t>
+  </si>
+  <si>
+    <t>CREDIAGIL</t>
+  </si>
+  <si>
+    <t>chipote95</t>
+  </si>
+  <si>
+    <t>29281026324</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -1263,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1276,10 +1300,10 @@
     <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1331,8 +1355,11 @@
       <c r="Q1" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -1364,8 +1391,11 @@
       <c r="Q2" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -1397,8 +1427,11 @@
       <c r="Q3" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1430,8 +1463,11 @@
       <c r="Q4" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="P9" s="14"/>
     </row>
   </sheetData>
@@ -1455,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1469,7 +1505,7 @@
     <col min="17" max="17" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1521,8 +1557,11 @@
       <c r="Q1" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -1554,8 +1593,11 @@
       <c r="Q2" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -1587,8 +1629,11 @@
       <c r="Q3" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1619,6 +1664,9 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7" t="s">
         <v>36</v>
+      </c>
+      <c r="R4" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1641,10 +1689,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1652,11 +1700,12 @@
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1708,8 +1757,11 @@
       <c r="Q1" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -1720,7 +1772,9 @@
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="8"/>
+      <c r="G2" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="H2" s="11">
         <v>1234</v>
       </c>
@@ -1730,15 +1784,20 @@
       <c r="J2" s="4"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="M2" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -1772,8 +1831,11 @@
       <c r="Q3" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1805,8 +1867,11 @@
       <c r="Q4" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="K5" s="13"/>
     </row>
   </sheetData>
@@ -1830,10 +1895,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1846,9 +1911,10 @@
     <col min="15" max="15" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1900,8 +1966,11 @@
       <c r="Q1" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -1929,8 +1998,11 @@
       <c r="Q2" s="10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -1962,8 +2034,11 @@
       <c r="Q3" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1993,8 +2068,11 @@
       <c r="Q4" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
@@ -2024,8 +2102,11 @@
       <c r="Q5" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
@@ -2057,8 +2138,11 @@
       <c r="Q6" s="10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="165">
+      <c r="R6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="165">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -2098,8 +2182,11 @@
       <c r="Q7" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
@@ -2131,11 +2218,14 @@
       <c r="Q8" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="14"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18">
       <c r="C11" s="13"/>
     </row>
   </sheetData>
@@ -2159,10 +2249,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2175,7 +2265,7 @@
     <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2227,8 +2317,11 @@
       <c r="Q1" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -2264,8 +2357,11 @@
       <c r="Q2" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -2299,11 +2395,14 @@
       <c r="Q3" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="13"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="N7" s="14"/>
     </row>
   </sheetData>

</xml_diff>